<commit_message>
Done with data splitting
</commit_message>
<xml_diff>
--- a/Source/Data/Final.xlsx
+++ b/Source/Data/Final.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="157">
   <si>
     <t>Model Name</t>
   </si>
@@ -485,112 +485,7 @@
     <t>Imperial Red Metallic, Mat Marvel Blue, Mat Axis Gray Metallic, Pearl Igneous Black, Pearl Deep Ground Gray</t>
   </si>
   <si>
-    <t>EV</t>
-  </si>
-  <si>
-    <t>Vehicle</t>
-  </si>
-  <si>
-    <t>Motor Power</t>
-  </si>
-  <si>
-    <t>Battery Type &amp; Capacity</t>
-  </si>
-  <si>
-    <t>Range (km)</t>
-  </si>
-  <si>
-    <t>Top Speed (km/h)</t>
-  </si>
-  <si>
-    <t>Charging Time</t>
-  </si>
-  <si>
-    <t>Tyres (Front/Rear)</t>
-  </si>
-  <si>
-    <t>Suspension (Front/Rear)</t>
-  </si>
-  <si>
-    <t>Technology &amp; Features</t>
-  </si>
-  <si>
-    <t>Colors</t>
-  </si>
-  <si>
-    <t>Warranty</t>
-  </si>
-  <si>
-    <t>Honda Activa e</t>
-  </si>
-  <si>
-    <t>6 kW PMSM motor</t>
-  </si>
-  <si>
-    <t>Swappable Li-ion, 1.5 kWh × 2 (total 3 kWh)</t>
-  </si>
-  <si>
-    <t>102 km/charge</t>
-  </si>
-  <si>
-    <t>80 km/h</t>
-  </si>
-  <si>
-    <t>7 hours (0–100%)</t>
-  </si>
-  <si>
-    <t>90/90-12 / 110/80-12</t>
-  </si>
-  <si>
-    <t>Front Disc 160 mm, Rear Drum 130 mm</t>
-  </si>
-  <si>
-    <t>Telescopic / Spring-loaded hydraulic (3-step)</t>
-  </si>
-  <si>
-    <t>Econ/Std/Sport modes, Reverse, Smart Key, TFT 7-inch RoadSync display</t>
-  </si>
-  <si>
-    <t>Pearl Shallow Blue, Pearl Misty White, Pearl Serenity Blue, Matt Foggy Silver, Pearl Igneous Black</t>
-  </si>
-  <si>
-    <t>3 years / 50,000 km</t>
-  </si>
-  <si>
-    <t>Honda QC1</t>
-  </si>
-  <si>
-    <t>1.8 kW hub motor</t>
-  </si>
-  <si>
-    <t>Fixed Li-ion, 1.5 kWh</t>
-  </si>
-  <si>
-    <t>80 km/charge</t>
-  </si>
-  <si>
-    <t>50 km/h</t>
-  </si>
-  <si>
-    <t>6.5 hours (0–100%)</t>
-  </si>
-  <si>
-    <t>12-inch alloy / 10-inch alloy</t>
-  </si>
-  <si>
-    <t>Front &amp; Rear Drum with CBS</t>
-  </si>
-  <si>
-    <t>Telescopic fork / Twin preload-adjustable shocks</t>
-  </si>
-  <si>
-    <t>LED lights, 5-inch LCD, USB-C, Econ &amp; Standard modes</t>
-  </si>
-  <si>
-    <t>Pearl Serenity Blue,Pearl Misty White,Matt Foggy Silver Metallic,Pearl Igneous Black,Pearl Shallow Blue</t>
-  </si>
-  <si>
-    <t>3 years (vehicle &amp; components)</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -598,7 +493,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -615,13 +510,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -679,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,22 +601,52 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1036,10 +967,10 @@
     <col min="9" max="9" style="5" width="56.43357142857143" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="5" width="51.14785714285715" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="5" width="67.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="88.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="21" width="88.57642857142856" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="5" width="109.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="22" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="22" width="14.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1121,16 +1052,16 @@
       <c r="K2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="3"/>
+      <c r="O2" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
@@ -1166,16 +1097,16 @@
       <c r="K3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="9" t="s">
         <v>73</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="3"/>
+      <c r="O3" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
@@ -1211,16 +1142,16 @@
       <c r="K4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="9" t="s">
         <v>86</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="3"/>
+      <c r="O4" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
@@ -1256,16 +1187,16 @@
       <c r="K5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="9" t="s">
         <v>97</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="O5" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
@@ -1301,16 +1232,16 @@
       <c r="K6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="9" t="s">
         <v>108</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="O6" s="3"/>
+      <c r="O6" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
@@ -1346,16 +1277,16 @@
       <c r="K7" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="9" t="s">
         <v>119</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="O7" s="3"/>
+      <c r="O7" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
@@ -1391,22 +1322,22 @@
       <c r="K8" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="9" t="s">
         <v>131</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="O8" s="3"/>
+      <c r="O8" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1436,22 +1367,22 @@
       <c r="K9" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="9" t="s">
         <v>145</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="O9" s="3"/>
+      <c r="O9" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1481,14 +1412,14 @@
       <c r="K10" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="9" t="s">
         <v>154</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3"/>
@@ -1502,10 +1433,10 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="L11" s="9"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3"/>
@@ -1519,16 +1450,16 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="8"/>
+      <c r="A13" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="13"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1538,137 +1469,137 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="9"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="1" t="s">
-        <v>157</v>
+      <c r="A14" s="14" t="s">
+        <v>156</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="C14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="10">
-      <c r="A16" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
+      <c r="A15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="17">
+      <c r="A16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="M16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1697,7 +1628,7 @@
     <col min="9" max="9" style="6" width="22.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1755,7 +1686,7 @@
         <v>112381</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1784,7 +1715,7 @@
         <v>112717</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1813,7 +1744,7 @@
         <v>124844</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1842,7 +1773,7 @@
         <v>128301</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1871,7 +1802,7 @@
         <v>126027</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1900,7 +1831,7 @@
         <v>107484</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1929,7 +1860,7 @@
         <v>121147</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1958,7 +1889,7 @@
         <v>131165</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1987,7 +1918,7 @@
         <v>142799</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -2016,7 +1947,7 @@
         <v>139074</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -2045,7 +1976,7 @@
         <v>128199</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
@@ -2074,7 +2005,7 @@
         <v>141264</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -2103,7 +2034,7 @@
         <v>93963</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -2132,7 +2063,7 @@
         <v>100122</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -2161,7 +2092,7 @@
         <v>111031</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -2190,7 +2121,7 @@
         <v>114282</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -2219,7 +2150,7 @@
         <v>112788</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -2248,7 +2179,7 @@
         <v>118253</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>

</xml_diff>